<commit_message>
Prepared to add to excel
</commit_message>
<xml_diff>
--- a/income_expenses.xlsx
+++ b/income_expenses.xlsx
@@ -432,14 +432,42 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Tipo de Pago</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Cantidad ($)</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Tipo de Pago</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Descripcion</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Prepared income page for adding things
</commit_message>
<xml_diff>
--- a/income_expenses.xlsx
+++ b/income_expenses.xlsx
@@ -414,14 +414,42 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Tipo de Pago</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Cantidad ($)</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Tipo de Pago</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Descripcion</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Prepared for test 4
</commit_message>
<xml_diff>
--- a/income_expenses.xlsx
+++ b/income_expenses.xlsx
@@ -450,11 +450,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Inscripcion de Jacobo Ganon Moragrega</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added Students Sheet to income_expenses.xlsx
</commit_message>
<xml_diff>
--- a/income_expenses.xlsx
+++ b/income_expenses.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Ingresos" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Egresos" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Estudiantes" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -449,9 +450,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-    </row>
+    <row r="2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -576,4 +575,22 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>